<commit_message>
Amended byars and wilson formulae when confidence = 1 or byars returns negative number.  associated amends to tests and documentation.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_Byars_Wilson.xlsx
+++ b/tests/testthat/testdata_Byars_Wilson.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgina.Anderson\Documents\R\Projects\PHEstatmethods\tests\testthat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgina.Anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
   <si>
     <t>95%</t>
   </si>
@@ -393,7 +393,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,14 +464,14 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>0.44500000000000001</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
-        <v>-5.3480593477991337E-3</v>
+        <v>1.3072132901504351E-2</v>
       </c>
       <c r="D4" s="4">
-        <v>4.5582829928092679</v>
+        <v>5.5637555824752605</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>0</v>
@@ -518,14 +518,14 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>0.44500000000000001</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4">
-        <v>-0.22261668693629325</v>
+        <v>2.916318374695686</v>
       </c>
       <c r="D7" s="4">
-        <v>8.1496882681862619</v>
+        <v>24.193724927880535</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>1</v>
@@ -655,11 +655,20 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="4">
+        <v>1</v>
+      </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
+      <c r="D14" s="4">
+        <v>9.362180217908362</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>

</xml_diff>